<commit_message>
changed member upload template
</commit_message>
<xml_diff>
--- a/public/docs/Members Template.xlsx
+++ b/public/docs/Members Template.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28619"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28803"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{77C2D549-EF68-436C-9EFA-6AC6282A7D32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{BF1E8B25-F9EA-4B70-8A0E-B0AA4CF22592}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -457,7 +457,7 @@
   <dimension ref="A1:M1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+      <selection activeCell="G2" sqref="G2:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -533,8 +533,8 @@
     <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid input" error="Member status can only be one of these: Active, Non-active, Moved away" promptTitle="Status" prompt="Active or Non-active or Moved away" sqref="F2:F1048576" xr:uid="{43ABCF89-B041-4B12-8C96-BE5F8427F971}">
       <formula1>"Active, Non-active, Moved away"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid input" error="Member role can only be some of these: Member, Non-member, Choir Official, NAGACU Official, NAGSDA, Departmental Leader, Elder, Pastor" promptTitle="Role" prompt="Member, Non-member, Choir Official or NAGACU Official or NAGSDA or Departmental Leader or Elder or Pastor" sqref="G2:G1048576" xr:uid="{707EF527-8F20-4FB2-AFFE-184B7676FE3A}">
-      <formula1>"Member, Non-member, Choir Official, NAGACU Official, NAGSDA, Departmental Leader, Elder, Pastor"</formula1>
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid input" error="Member role can only be some of these: Member, Local Church Ministry Leader, NAGSDA Official, Departmental Leader, Local Church Elder, Pastor, Non-member, Non-Member (Guest), Non-Adventist (Guest)" promptTitle="Role" prompt="Member or Local Church Ministry Leader or NAGSDA Official or Departmental Leader or Local Church Elder or Pastor or Non-member or Non-Member (Guest) or Non-Adventist (Guest)" sqref="G2:G1048576" xr:uid="{707EF527-8F20-4FB2-AFFE-184B7676FE3A}">
+      <formula1>"Member, Local Church Ministry Leader, NAGSDA Official, Departmental Leader, Local Church Elder, Pastor, Non-member, Non-Member (Guest), Non-Adventist (Guest)"</formula1>
     </dataValidation>
     <dataValidation type="textLength" operator="greaterThanOrEqual" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid input" error="Enter a valid name. Name must be at least 6 characters" promptTitle="Name" prompt="Must be at least 6 characters" sqref="A2:A1048576" xr:uid="{CFCA2F22-9F48-4C5D-AFCC-353EA6E10BC2}">
       <formula1>6</formula1>

</xml_diff>